<commit_message>
Apache POI 07 Question added Multiplation Table
08 Creating an Excel File in the directory
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resources/WriteInTheExcelFile.xlsx
+++ b/src/test/java/ApachePOI/resources/WriteInTheExcelFile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TechnoStudy\IdeaProjects\Cucumber7\src\test\java\ApachePOI\resource\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,11 +24,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Merhaba</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -347,7 +352,13 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>